<commit_message>
HELL YEAHHH 90% PROGRESS
</commit_message>
<xml_diff>
--- a/data/ngolist.xlsx
+++ b/data/ngolist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\DjangoProjects\nasom-job-portal\nasom_job_portal\verify_applicant\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\DjangoProjects\nasom-job-portal\nasom_job_portal\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F312BB-DA31-43D7-B597-7A5133EC3E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6361CD72-8495-4313-902A-ABFFFD319228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>NASOM Setia Alam</t>
   </si>
@@ -33,94 +33,49 @@
     <t>NASOM Gombak</t>
   </si>
   <si>
-    <t>gombak@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Taman Supreme</t>
   </si>
   <si>
-    <t>supreme@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Jalan Ipoh</t>
   </si>
   <si>
-    <t>kljalanipoh@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Teluk Pulai</t>
   </si>
   <si>
-    <t>telukpulai@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Titiwangsa</t>
   </si>
   <si>
-    <t>titiwangsa@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Bandar Puteri</t>
   </si>
   <si>
-    <t>vocklang@nasom.org.my</t>
-  </si>
-  <si>
-    <t>NASOM AYAC (Klang)</t>
-  </si>
-  <si>
-    <t>ayacklang@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Penang</t>
   </si>
   <si>
-    <t>penang@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Alor Setar</t>
   </si>
   <si>
-    <t>kedah@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Ipoh</t>
   </si>
   <si>
-    <t>ipoh@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Butterworth</t>
   </si>
   <si>
-    <t>butterworth@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Melaka</t>
   </si>
   <si>
-    <t>melaka@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Kuantan</t>
   </si>
   <si>
     <t>NASOM Kerteh</t>
   </si>
   <si>
-    <t>kerteh@nasom.org.my</t>
-  </si>
-  <si>
     <t>NASOM Kota Kinabalu</t>
   </si>
   <si>
-    <t>kotakinabalu@nasom.org.my</t>
-  </si>
-  <si>
-    <t>cac@nasom.org.my</t>
-  </si>
-  <si>
-    <t>kuantan@nasom.org.my</t>
+    <t>2022882978@student.uitm.edu.my</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NASOM AYAC </t>
   </si>
 </sst>
 </file>
@@ -457,161 +412,153 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:gombak@nasom.org.my" xr:uid="{2071D06D-4327-43FC-AD31-ED5374618F31}"/>
-    <hyperlink ref="B3" r:id="rId2" display="mailto:supreme@nasom.org.my" xr:uid="{E52519A9-FD73-46DD-AD75-AFC9C4EE9BF7}"/>
-    <hyperlink ref="B4" r:id="rId3" display="mailto:kljalanipoh@nasom.org.my" xr:uid="{E1A2FCF8-0C86-4DE6-B2D5-34F869E32A6E}"/>
-    <hyperlink ref="B5" r:id="rId4" display="mailto:telukpulai@nasom.org.my" xr:uid="{B16D19C2-732B-44D4-B514-9EF977000B01}"/>
-    <hyperlink ref="B6" r:id="rId5" display="mailto:titiwangsa@nasom.org.my" xr:uid="{E45E12DE-FD86-4BE7-93C3-167F84F7187B}"/>
-    <hyperlink ref="B7" r:id="rId6" display="mailto:vocklang@nasom.org.my" xr:uid="{F36229F1-8362-4A4C-8FC8-C461709F0343}"/>
-    <hyperlink ref="B8" r:id="rId7" display="mailto:ayacklang@nasom.org.my" xr:uid="{C5849B46-FB86-4078-AB53-AD0177452EF7}"/>
-    <hyperlink ref="B9" r:id="rId8" display="mailto:penang@nasom.org.my" xr:uid="{B04D89C0-2F77-4773-B141-DD983E63061C}"/>
-    <hyperlink ref="B10" r:id="rId9" display="mailto:kedah@nasom.org.my" xr:uid="{B6E80594-B18A-4CCC-9FE1-7BA4C70EAA37}"/>
-    <hyperlink ref="B11" r:id="rId10" display="mailto:ipoh@nasom.org.my" xr:uid="{5F165A88-6C3B-435E-B404-FC31A0629EB5}"/>
-    <hyperlink ref="B12" r:id="rId11" display="mailto:butterworth@nasom.org.my" xr:uid="{8D509A81-E418-4909-A8BC-7706822E2A0D}"/>
-    <hyperlink ref="B13" r:id="rId12" display="mailto:melaka@nasom.org.my" xr:uid="{C590E9C6-4F4C-45CA-83FD-AF0453DE548B}"/>
-    <hyperlink ref="B15" r:id="rId13" display="mailto:kerteh@nasom.org.my" xr:uid="{C285F130-6722-47AC-9E60-C807D936E7B6}"/>
-    <hyperlink ref="B16" r:id="rId14" display="mailto:kotakinabalu@nasom.org.my" xr:uid="{92E2A346-EFEF-4576-AFC5-034A9C9A8CFE}"/>
-    <hyperlink ref="B1" r:id="rId15" xr:uid="{C097C657-DDBC-48F6-A2B8-39F914251D71}"/>
-    <hyperlink ref="B14" r:id="rId16" xr:uid="{2751967A-AD3B-446D-8AF9-7E6BB232AA73}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{C097C657-DDBC-48F6-A2B8-39F914251D71}"/>
+    <hyperlink ref="B2:B4" r:id="rId2" display="2022882978@student.uitm.edu.my" xr:uid="{6BA81152-8D3F-477F-B285-68CF3439060A}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{7DDE039E-409C-4226-A745-FDA572686F21}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{45D50A50-0E81-49D3-B8DD-B1EFDB7B82B1}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{807AFA40-44F2-4CCB-BDF4-7EFFC7C66485}"/>
+    <hyperlink ref="B6:B8" r:id="rId6" display="2022882978@student.uitm.edu.my" xr:uid="{4F0E2972-BDA9-4CE8-926D-EFC9BBF4BEE0}"/>
+    <hyperlink ref="B10:B12" r:id="rId7" display="2022882978@student.uitm.edu.my" xr:uid="{5013970A-46A3-4867-995C-81726FDB6AA1}"/>
+    <hyperlink ref="B14:B16" r:id="rId8" display="2022882978@student.uitm.edu.my" xr:uid="{751AAE72-4784-4E6C-A61E-D495995AC9E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>